<commit_message>
classified all files, hopefully
</commit_message>
<xml_diff>
--- a/Warehouse/AA/judgement_logs_run4o.xlsx
+++ b/Warehouse/AA/judgement_logs_run4o.xlsx
@@ -462,13 +462,13 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie."
+MSG: The decision has been recorded with no movie chosen for Friday.
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -484,13 +484,13 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights to "Barbie" have been successfully acquired for the upcoming assembly.
+MSG: The decision process has concluded without an agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -506,13 +506,13 @@
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday could not be made.
 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -528,13 +528,13 @@
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie selected for Friday based on the committee's discussion.
 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the upcoming assembly.
+MSG: The decision has been recorded to acquire the rights to show "Barbie" on Friday.
 </t>
         </is>
       </c>
@@ -572,13 +572,13 @@
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" based on the committee's discussions.
+MSG: The decision process resulted in no agreement on which movie to play, leading to the conclusion of no decision being made.
 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -594,13 +594,13 @@
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no agreement was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -616,13 +616,13 @@
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The committee did not arrive at a decision regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -638,13 +638,13 @@
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming screening based on the committee's discussion and votes.
+MSG: The decision process concluded without a clear agreement on which movie to show on Friday, resulting in no movie selection.
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -660,13 +660,13 @@
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for the upcoming event.
+MSG: The decision to show a movie on Friday could not be reached, and thus, no acquisition will be made.
 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -682,13 +682,13 @@
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the assembly on Friday.
+MSG: The function has been called, indicating that no decision about Friday’s movie has been made.
 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -704,13 +704,13 @@
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the screening on Friday.
+MSG: The decision about which movie to play on Friday was not reached, so I have recorded that there was no decision made.
 </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -726,13 +726,13 @@
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Barbie" as the movie that will be shown on Friday.
+MSG: The rights for both movies have been acquired.
 </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -748,13 +748,13 @@
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding the movie to be shown on Friday was reached.
 </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been recorded. "Oppenheimer" will be shown on Friday.
 </t>
         </is>
       </c>
@@ -792,13 +792,13 @@
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the event on Friday.
+MSG: The decision has been recorded as no movie was selected.
 </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -814,13 +814,13 @@
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Oppenheimer" for the movie to be shown on Friday.
+MSG: The decision about which movie to show on Friday was not reached.
 </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -836,13 +836,13 @@
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision about which movie to show on Friday could not be made.
 </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -858,13 +858,13 @@
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights to show "Oppenheimer" for the event.
+MSG: The decision has been recorded as no decision about Friday's movie can be made.
 </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -880,13 +880,13 @@
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as a no decision regarding the movie selection for Friday.
 </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -902,13 +902,13 @@
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Oppenheimer" based on its emphasis on fostering critical discussions and preparing students for the complexities they will encounter in adulthood.
+MSG: The decision about which movie to show on Friday was not reached, so no acquisition will be made.
 </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -924,13 +924,13 @@
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision process has concluded without a definitive choice for Friday's movie, resulting in no movie being selected.
 </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -946,13 +946,13 @@
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming screening.
+MSG: The committee did not reach a decision regarding the movie to show on Friday, so the outcome is recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been finalized, as it is the selected movie for Friday’s screening.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -990,13 +990,13 @@
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" on Friday.
+MSG: The decision regarding which movie to show on Friday has not been finalized.
 </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1012,13 +1012,13 @@
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights to "Barbie" for the screening based on the conversation in the committee meeting.
+MSG: The decision has been recorded as no decision about Friday's movie can be made.
 </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1034,13 +1034,13 @@
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as "no decision" regarding the selection of a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights for both movies, "Oppenheimer" and "Barbie," to be shown in their entirety on Friday.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
@@ -1078,13 +1078,13 @@
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie was selected in the discussion.
 </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," which will be shown during the event on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1122,13 +1122,13 @@
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Barbie" for the movie showing on Friday.
+MSG: The decision has been recorded. There is no agreement on which movie to show on Friday, so the conversation has concluded without a plan.
 </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to show on Friday.
+MSG: The decision has been recorded: "Oppenheimer" was selected to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1166,13 +1166,13 @@
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1210,13 +1210,13 @@
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for Friday's movie presentation.
+MSG: The decision has been recorded as no selection being made for Friday's movie.
 </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1232,13 +1232,13 @@
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown during the assembly.
+MSG: The decision has been recorded as no movie selected for this meeting.
 </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1254,13 +1254,13 @@
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been recorded as there being no decision about the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1276,13 +1276,13 @@
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision-making process concluded without a clear choice for Friday's movie, so no decision was made.
 </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1298,13 +1298,13 @@
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The function has been called, and the decision reflects that the committee could not reach an agreement on a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1342,13 +1342,13 @@
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the public performance rights for "Barbie."
+MSG: The decision regarding the movie for Friday was not made.
 </t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded and the rights to "Barbie" have been acquired for Friday's movie showing.
 </t>
         </is>
       </c>
@@ -1386,13 +1386,13 @@
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights to "Barbie" have been successfully acquired for the screening.
+MSG: A decision was not reached regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1408,13 +1408,13 @@
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been recorded.
+MSG: The decision has been registered as "no decision," indicating that there was no consensus reached about which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -1452,13 +1452,13 @@
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Barbie" for the event on Friday.
+MSG: The decision has been recorded, indicating that no agreement was reached regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1474,13 +1474,13 @@
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded with no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1496,13 +1496,13 @@
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision regarding the movie to be shown on Friday has been concluded with no selection made.
 </t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1518,7 +1518,7 @@
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights to show "Barbie" during the event.
+MSG: The decision to show "Barbie" has been successfully made.
 </t>
         </is>
       </c>
@@ -1540,13 +1540,13 @@
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The conversation concluded without a decision regarding what movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1562,13 +1562,13 @@
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday, reflecting the committee's consensus to combine enjoyment and educational value for the event.
+MSG: I've successfully acquired the rights for both movies.
 </t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1584,13 +1584,13 @@
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be screened on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1606,13 +1606,13 @@
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the movie to be shown on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1628,13 +1628,13 @@
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, indicating that no choice of movie can be made at this time.
 </t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie."
+MSG: The decision has been recorded, and the movie "Barbie" will be acquired for showing this Friday.
 </t>
         </is>
       </c>
@@ -1672,13 +1672,13 @@
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision regarding which movie to show on Friday has been recorded as "no decision."
 </t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1694,13 +1694,13 @@
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer," which will be shown at the upcoming assembly.
+MSG: The rights for both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1716,13 +1716,13 @@
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" on Friday.
+MSG: The result indicates that there was no decision made regarding the movie selection for Friday.
 </t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1738,13 +1738,13 @@
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision about which movie to show on Friday remains unresolved, as indicated by the lack of consensus between the committee members.
 </t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1760,13 +1760,13 @@
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision-making process has reached a point of no consensus regarding the movie for Friday, and thus, no decision has been made.
 </t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1782,13 +1782,13 @@
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event on Friday.
+MSG: The decision process has concluded without a selection for the movie to be shown on Friday. No movie rights will be acquired at this time.
 </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision is made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1826,13 +1826,13 @@
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights to both movies, "Oppenheimer" and "Barbie," for the screening on Friday.
+MSG: The decision has been recorded, and no specific movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1848,13 +1848,13 @@
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the public performance rights for "Barbie."
+MSG: The decision has been recorded as a no decision regarding which movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1870,13 +1870,13 @@
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event.
+MSG: The decision to show a movie on Friday remains undecided, as there was no agreement reached during the conversation.
 </t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1892,13 +1892,13 @@
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie." This choice reflects the committee's emphasis on finding a film that resonates well with the seniors and fosters meaningful discussions.
+MSG: The decision process regarding the movie for Friday concluded without reaching a definitive agreement, so no decision has been made.
 </t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming event on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1936,13 +1936,13 @@
       <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding which movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1958,7 +1958,7 @@
       <c r="C70" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="C71" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for the movie "Barbie."
 </t>
         </is>
       </c>
@@ -2002,13 +2002,13 @@
       <c r="C72" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2024,13 +2024,13 @@
       <c r="C73" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event on Friday.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       <c r="C74" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and the movie "Barbie" will be acquired for Friday's showing.
 </t>
         </is>
       </c>
@@ -2068,13 +2068,13 @@
       <c r="C75" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2090,13 +2090,13 @@
       <c r="C76" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been made: there was no consensus on which movie to select for Friday's viewing, so no decision will be recorded.
 </t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2112,13 +2112,13 @@
       <c r="C77" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision have been recorded as no decision was made about which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2134,7 +2134,7 @@
       <c r="C78" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the event.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -2156,13 +2156,13 @@
       <c r="C79" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The committee did not reach a decision regarding which movie to show on Friday, so no further action can be taken.
 </t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2178,13 +2178,13 @@
       <c r="C80" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no agreement was reached on a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
       <c r="C81" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Oppenheimer" to be shown at the upcoming event on Friday.
+MSG: The decision to show "Oppenheimer" has been recorded successfully.
 </t>
         </is>
       </c>
@@ -2222,13 +2222,13 @@
       <c r="C82" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The committee did not reach a decision on which movie to show on Friday, so no film will be acquired at this time.
 </t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2244,7 +2244,7 @@
       <c r="C83" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -2266,13 +2266,13 @@
       <c r="C84" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision has been recorded as no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2288,13 +2288,13 @@
       <c r="C85" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to show on Friday.
+MSG: The decision process about the movie for Friday ended without a clear choice, so no acquisition is made.
 </t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       <c r="C86" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not reach a concrete decision regarding which movie will be shown on Friday, as they opted to poll the students for their preferences. Thus, I will call the no_decision function.
+MSG: The decision has been recorded as "no decision."
 </t>
         </is>
       </c>
@@ -2332,13 +2332,13 @@
       <c r="C87" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2354,13 +2354,13 @@
       <c r="C88" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Oppenheimer" based on the committee's agreement to showcase this film for the event on Friday.
+MSG: The decision has been made to acquire the rights for both movies.
 </t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2376,13 +2376,13 @@
       <c r="C89" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming screening.
+MSG: The decision has been recorded as "no decision."
 </t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2398,7 +2398,7 @@
       <c r="C90" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision to acquire the rights for "Oppenheimer" has been successfully recorded. The movie will be shown on Friday. 
 </t>
         </is>
       </c>
@@ -2420,13 +2420,13 @@
       <c r="C91" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2442,13 +2442,13 @@
       <c r="C92" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for the upcoming event.
+MSG: The decision process has concluded without a clear choice for a movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       <c r="C93" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the rights for "Barbie" have been acquired for the screening on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -2508,13 +2508,13 @@
       <c r="C95" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2530,13 +2530,13 @@
       <c r="C96" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2552,13 +2552,13 @@
       <c r="C97" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for the movie "Oppenheimer."
+MSG: The decision process concluded without a selected movie for Friday, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2574,13 +2574,13 @@
       <c r="C98" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision to acquire the rights for both movies has been successfully made.
 </t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2596,13 +2596,13 @@
       <c r="C99" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" based on the conversation and sentiments expressed during the committee meeting.
+MSG: The decision regarding the movie for Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2618,13 +2618,13 @@
       <c r="C100" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision was made regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2640,13 +2640,13 @@
       <c r="C101" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been noted as "no decision" regarding which movie to acquire for Friday.
 </t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2662,13 +2662,13 @@
       <c r="C102" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: I have recorded the decision as "no_decision" since the committee did not arrive at a specific choice for Friday's movie.
 </t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2684,7 +2684,7 @@
       <c r="C103" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision to show "Barbie" on Friday has been confirmed.
 </t>
         </is>
       </c>
@@ -2706,13 +2706,13 @@
       <c r="C104" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the event.
+MSG: The decision process concluded without selecting a movie for Friday, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2728,13 +2728,13 @@
       <c r="C105" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision to acquire rights for both movies has been executed.
 </t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2750,13 +2750,13 @@
       <c r="C106" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision-making process did not result in a final choice for Friday's movie.
 </t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2772,13 +2772,13 @@
       <c r="C107" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Oppenheimer" on Friday.
+MSG: The decision has been recorded as no consensus was reached regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2794,13 +2794,13 @@
       <c r="C108" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision from the committee is that no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2816,13 +2816,13 @@
       <c r="C109" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2838,13 +2838,13 @@
       <c r="C110" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision about which movie to play on Friday could not be made, as there was no consensus reached.
 </t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2860,13 +2860,13 @@
       <c r="C111" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2882,13 +2882,13 @@
       <c r="C112" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2904,13 +2904,13 @@
       <c r="C113" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the screening on Friday.
+MSG: The decision process did not result in an agreement on which movie to show on Friday, so the outcome is recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2926,13 +2926,13 @@
       <c r="C114" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as "no decision" regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2948,13 +2948,13 @@
       <c r="C115" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights to show "Oppenheimer" on Friday.
+MSG: The decision about the movie for Friday has been recorded as "no decision."
 </t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -2970,13 +2970,13 @@
       <c r="C116" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The rights for both "Oppenheimer" and "Barbie" have been acquired for Friday's movie showing.
 </t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -2992,13 +2992,13 @@
       <c r="C117" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3014,13 +3014,13 @@
       <c r="C118" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The function for no decision has been successfully called, indicating that there was no agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3036,13 +3036,13 @@
       <c r="C119" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision regarding the movie for Friday has concluded without a selection being made.
 </t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3058,13 +3058,13 @@
       <c r="C120" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for Friday's movie showing.
+MSG: The committee did not reach a decision on which movie to show on Friday, so the outcome was recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3080,13 +3080,13 @@
       <c r="C121" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision process concluded without making a choice for Friday's movie, so no selection was made.
 </t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3102,13 +3102,13 @@
       <c r="C122" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Barbie."
+MSG: The decision regarding the movie to show on Friday ended without a conclusion, so no action will be taken to acquire rights for any film.
 </t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3124,13 +3124,13 @@
       <c r="C123" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision regarding which movie to show on Friday has been recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3146,13 +3146,13 @@
       <c r="C124" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie."
+MSG: The decision has been recorded as no decision regarding Friday's movie.
 </t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3168,13 +3168,13 @@
       <c r="C125" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -3190,13 +3190,13 @@
       <c r="C126" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the screening on Friday.
+MSG: The decision-making discussion did not lead to a conclusion on which movie to show on Friday, so the outcome is that no decision was reached.
 </t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3212,13 +3212,13 @@
       <c r="C127" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3234,7 +3234,7 @@
       <c r="C128" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded: "Barbie" will be the movie selected for the event.
+MSG: The rights to "Barbie" have been successfully acquired for Friday's showing.
 </t>
         </is>
       </c>
@@ -3256,13 +3256,13 @@
       <c r="C129" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3278,13 +3278,13 @@
       <c r="C130" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -3300,13 +3300,13 @@
       <c r="C131" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The rights for both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -3322,13 +3322,13 @@
       <c r="C132" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday was not made.
 </t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3344,13 +3344,13 @@
       <c r="C133" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming student event.
+MSG: The decision about which movie to show on Friday remains unresolved.
 </t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       <c r="C134" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for Friday’s event.
+MSG: The decision has been recorded, and the rights for "Oppenheimer" will be acquired.
 </t>
         </is>
       </c>
@@ -3388,13 +3388,13 @@
       <c r="C135" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: I have recorded the decision as no_decision.
 </t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3410,7 +3410,7 @@
       <c r="C136" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded successfully. The movie "Barbie" will be acquired for the assembly on Friday.
 </t>
         </is>
       </c>
@@ -3432,13 +3432,13 @@
       <c r="C137" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: I have recorded the decision to acquire the rights for both movies.
 </t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -3454,13 +3454,13 @@
       <c r="C138" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday as part of the graduation event.
+MSG: The decision-making process did not result in a choice for Friday's movie, leading to a no decision outcome.
 </t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3476,13 +3476,13 @@
       <c r="C139" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision regarding the movie to be shown on Friday has resulted in no selection being made.
 </t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3498,13 +3498,13 @@
       <c r="C140" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for “Barbie” to be shown on Friday.
+MSG: The decision resulted in no agreement on what movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
       <c r="C141" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," which will be shown in the assembly.
+MSG: The decision has been recorded to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -3542,13 +3542,13 @@
       <c r="C142" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming screening on Friday.
+MSG: The decision has been made to acquire the rights to both movies.
 </t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -3564,13 +3564,13 @@
       <c r="C143" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming event.
+MSG: The decision regarding the movie for Friday was not finalized, resulting in no selection being made.
 </t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3586,13 +3586,13 @@
       <c r="C144" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for Friday's showing.
+MSG: The decision regarding which movie to play on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3608,13 +3608,13 @@
       <c r="C145" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer" for the upcoming event.
+MSG: The decision regarding which movie to show on Friday resulted in no consensus. The choice has been marked as "no decision".
 </t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3630,13 +3630,13 @@
       <c r="C146" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Barbie" to be shown at the graduation event on Friday.
+MSG: The decision about which movie to show on Friday was not made.
 </t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3652,13 +3652,13 @@
       <c r="C147" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision to show a movie on Friday was not finalized, so I will record that no decision was made regarding the movie selection.
 </t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3674,13 +3674,13 @@
       <c r="C148" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the upcoming event.
+MSG: The decision regarding Friday's movie could not be made, and therefore, the call for the function has successfully reflected that outcome.
 </t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3696,13 +3696,13 @@
       <c r="C149" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming student assembly.
+MSG: The decision has been recorded as no decision was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3718,7 +3718,7 @@
       <c r="C150" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown during Friday's event.
+MSG: I have recorded the decision to acquire the rights to "Barbie" for the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -3740,13 +3740,13 @@
       <c r="C151" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Barbie" after considering the committee's discussions and the emphasis on engagement and positivity for the students. The film aligns well with the objectives of fostering creativity and open discussions.
+MSG: The committee did not reach a decision regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3762,7 +3762,7 @@
       <c r="C152" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the assembly.
+MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -3784,13 +3784,13 @@
       <c r="C153" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for Friday's movie screening.
+MSG: The decision-making process concluded without an agreement on which movie to show, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3806,13 +3806,13 @@
       <c r="C154" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the public performance rights for "Oppenheimer" has been recorded successfully.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3828,13 +3828,13 @@
       <c r="C155" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been made to not acquire any movie rights at this time, as there was no consensus reached regarding the movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3850,13 +3850,13 @@
       <c r="C156" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for the movie showing on Friday.
+MSG: The decision has been recorded as no movie was selected during the meeting.
 </t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3872,13 +3872,13 @@
       <c r="C157" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," as it aligns well with the themes discussed by the committee and is expected to provide an engaging experience for the students.
+MSG: No decision was made regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3894,13 +3894,13 @@
       <c r="C158" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision process has concluded with no specific movie chosen for Friday.
 </t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3916,13 +3916,13 @@
       <c r="C159" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the public performance rights for "Oppenheimer."
+MSG: The decision regarding which movie to show on Friday is considered to have no conclusion at this time.
 </t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3938,13 +3938,13 @@
       <c r="C160" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for the movie **“Barbie.”**
+MSG: The decision on which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3960,13 +3960,13 @@
       <c r="C161" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -3982,7 +3982,7 @@
       <c r="C162" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," which will be shown at the event for the seniors.
+MSG: The decision has been recorded, and "Barbie" will be shown on Friday.
 </t>
         </is>
       </c>
@@ -4004,13 +4004,13 @@
       <c r="C163" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for both movies, "Barbie" and "Oppenheimer," as they will be shown in their entirety during the event.
+MSG: The decision has been recorded, indicating that no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4026,13 +4026,13 @@
       <c r="C164" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4048,7 +4048,7 @@
       <c r="C165" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie that will be shown on Friday.
+MSG: The decision has been made to select the movie "Barbie" for the meeting.
 </t>
         </is>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="C166" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to both movies "Barbie" and "Oppenheimer" for the upcoming event.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
@@ -4092,13 +4092,13 @@
       <c r="C167" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4114,13 +4114,13 @@
       <c r="C168" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights to show "Oppenheimer" on Friday.
+MSG: The decision regarding the movie for Friday has concluded without a selection.
 </t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4136,13 +4136,13 @@
       <c r="C169" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about Friday's movie has ended without a plan, resulting in no selection.
 </t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4158,13 +4158,13 @@
       <c r="C170" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the senior assembly.
+MSG: The decision process concluded without selecting a movie for Friday. No movie rights will be acquired at this time.
 </t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4180,13 +4180,13 @@
       <c r="C171" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming student event. The film aligns well with the emotional and developmental needs of the students.
+MSG: The decision about Friday's movie will not be made at this time.
 </t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4202,7 +4202,7 @@
       <c r="C172" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision has been recorded, and rights for "Barbie" will be acquired.
 </t>
         </is>
       </c>
@@ -4224,13 +4224,13 @@
       <c r="C173" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision regarding what movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4246,13 +4246,13 @@
       <c r="C174" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for “Barbie.”
+MSG: The decision process resulted in no agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4268,13 +4268,13 @@
       <c r="C175" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is made to acquire the rights for both "Barbie" and "Oppenheimer" as the committee intends to present both movies to the students for their feedback and participation in deciding which film resonates more with them.
+MSG: The decision about which movie to show on Friday has not been made, resulting in no decision being recorded.
 </t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4290,13 +4290,13 @@
       <c r="C176" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been made, and no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4312,13 +4312,13 @@
       <c r="C177" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming assembly on Friday.
+MSG: The decision regarding the movie for Friday was not made.
 </t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4334,7 +4334,7 @@
       <c r="C178" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the event on Friday.
+MSG: I have recorded the decision to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -4356,13 +4356,13 @@
       <c r="C179" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded as no decision was made regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4378,13 +4378,13 @@
       <c r="C180" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" based on the committee's discussions.
+MSG: The committee did not reach a decision about which movie to show on Friday, so there will be no movie acquired.
 </t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4400,13 +4400,13 @@
       <c r="C181" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming Friday screening.
+MSG: The decision regarding the movie for Friday was not made, as the committee did not reach a consensus.
 </t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4422,7 +4422,7 @@
       <c r="C182" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Oppenheimer," which will be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -4444,7 +4444,7 @@
       <c r="C183" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for the movie "Barbie."
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -4466,13 +4466,13 @@
       <c r="C184" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision-making process ended without a clear agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4488,13 +4488,13 @@
       <c r="C185" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: No decision was made regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4510,13 +4510,13 @@
       <c r="C186" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Oppenheimer" for the upcoming event.
+MSG: The decision about Friday's movie cannot be made.
 </t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4532,13 +4532,13 @@
       <c r="C187" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to show on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4554,13 +4554,13 @@
       <c r="C188" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision regarding the movie to be shown on Friday has not been made, so we have no conclusion to act upon.
 </t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4576,7 +4576,7 @@
       <c r="C189" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee reached no decision regarding the movie selection for Friday, as they were unable to come to a consensus between "Barbie" and "Oppenheimer."
+MSG: The decision has been recorded: no final choice about Friday's movie was made.
 </t>
         </is>
       </c>
@@ -4598,13 +4598,13 @@
       <c r="C190" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision about which movie to show on Friday was not reached.
 </t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4620,13 +4620,13 @@
       <c r="C191" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4642,13 +4642,13 @@
       <c r="C192" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision regarding the movie to be shown on Friday has been recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4664,13 +4664,13 @@
       <c r="C193" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision about what movie to show on Friday was not reached, and thus no selection was made.
 </t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4686,13 +4686,13 @@
       <c r="C194" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The committee did not reach a decision regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4708,13 +4708,13 @@
       <c r="C195" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights to "Barbie" has been made, as it will be shown during Friday's event.
+MSG: The decision was made to not select a movie for Friday, as there was no definitive agreement reached.
 </t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4730,13 +4730,13 @@
       <c r="C196" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no movie was chosen.
 </t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4752,13 +4752,13 @@
       <c r="C197" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision-making process did not lead to an agreement about which movie to show on Friday, hence no action was taken.
 </t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4774,13 +4774,13 @@
       <c r="C198" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for the upcoming student assembly.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4796,13 +4796,13 @@
       <c r="C199" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer" as the featured film for the upcoming event.
+MSG: The rights to both movies have been acquired for Friday.
 </t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -4818,13 +4818,13 @@
       <c r="C200" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event on Friday.
+MSG: The decision has been recorded as no decision regarding Friday's movie was made.
 </t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4840,13 +4840,13 @@
       <c r="C201" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for the movie "Oppenheimer."
+MSG: The decision has been recorded as no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4862,13 +4862,13 @@
       <c r="C202" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been processed, and it has been recorded that no movie was selected for screening.
 </t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4884,13 +4884,13 @@
       <c r="C203" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision process did not result in a clear choice for Friday's movie, and therefore, no decision was made.
 </t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4906,13 +4906,13 @@
       <c r="C204" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming event on Friday.
+MSG: The decision for the movie to be shown on Friday has been noted as no decision.
 </t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4928,13 +4928,13 @@
       <c r="C205" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire public performance rights for "Oppenheimer."
+MSG: The decision has been recorded as no decision about Friday's movie can be made.
 </t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4950,13 +4950,13 @@
       <c r="C206" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for Friday's event.
+MSG: I have recorded the decision as no consensus was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -4972,7 +4972,7 @@
       <c r="C207" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for both "Barbie" and "Oppenheimer" for the upcoming movie screening.
+MSG: The decision to acquire the rights for both movies has been recorded successfully.
 </t>
         </is>
       </c>
@@ -4994,13 +4994,13 @@
       <c r="C208" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision has been recorded, and no movie has been selected for Friday.
 </t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5016,13 +5016,13 @@
       <c r="C209" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming screening.
+MSG: The decision-making process regarding the movie selection concluded without a specific choice being made.
 </t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5038,13 +5038,13 @@
       <c r="C210" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to show it on Friday.
+MSG: The decision about which movie to show on Friday has not been made, as the committee did not reach an agreement.
 </t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5060,13 +5060,13 @@
       <c r="C211" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The rights for both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       <c r="C212" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," which will be shown at the school assembly on Friday.
+MSG: The decision has been recorded, and the movie "Barbie" will be acquired.
 </t>
         </is>
       </c>
@@ -5104,13 +5104,13 @@
       <c r="C213" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The committee did not reach an agreement on which movie to show, leading to the decision of no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
       <c r="C214" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie," which will be shown on Friday.
+MSG: The decision has been made to acquire the rights to "Barbie" for the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -5148,13 +5148,13 @@
       <c r="C215" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded as "no_decision," indicating that the committee did not reach an agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5170,13 +5170,13 @@
       <c r="C216" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Barbie" for the film screening on Friday.
+MSG: The decision was made to not select a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5192,13 +5192,13 @@
       <c r="C217" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about what movie to show on Friday could not be made, as there was no consensus reached by the committee.
 </t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5214,13 +5214,13 @@
       <c r="C218" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no movie was chosen for Friday.
 </t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5236,13 +5236,13 @@
       <c r="C219" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie."
+MSG: The decision has been recorded with no selected movie for Friday.
 </t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5258,13 +5258,13 @@
       <c r="C220" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision was reached regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5280,13 +5280,13 @@
       <c r="C221" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the movie shown on Friday.
+MSG: I have decided to acquire the rights to both movies.
 </t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5302,7 +5302,7 @@
       <c r="C222" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for both "Barbie" and "Oppenheimer" for the screening and discussions planned for Friday.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
@@ -5324,13 +5324,13 @@
       <c r="C223" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Barbie" based on the committee's discussion and focus on student engagement and inspiration for the event.
+MSG: The committee did not arrive at a decision regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5346,13 +5346,13 @@
       <c r="C224" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision has been recorded with no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5368,7 +5368,7 @@
       <c r="C225" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer" for the screening event on Friday.
+MSG: The decision to show "Oppenheimer" on Friday has been confirmed.
 </t>
         </is>
       </c>
@@ -5390,13 +5390,13 @@
       <c r="C226" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision to acquire the rights for both movies has been successfully recorded.
 </t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5412,13 +5412,13 @@
       <c r="C227" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision has been recorded, and no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5434,13 +5434,13 @@
       <c r="C228" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming assembly.
+MSG: The decision process has concluded without arriving at an agreement on which movie to show, so no further actions will be taken.
 </t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5456,13 +5456,13 @@
       <c r="C229" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded and there will be no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5478,13 +5478,13 @@
       <c r="C230" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer."
+MSG: The rights to both movies have been acquired.
 </t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5500,7 +5500,7 @@
       <c r="C231" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be screened on Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -5522,13 +5522,13 @@
       <c r="C232" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been made, and it will be shown at the upcoming student event.
+MSG: The decision has been recorded as no choice of a movie was made during the discussion.
 </t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5544,13 +5544,13 @@
       <c r="C233" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming event.
+MSG: The decision to acquire a movie for Friday was not reached, so no further action will be taken.
 </t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5566,13 +5566,13 @@
       <c r="C234" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The rights to both "Oppenheimer" and "Barbie" have been acquired for Friday's screening.
 </t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5588,13 +5588,13 @@
       <c r="C235" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Oppenheimer" has been recorded.
+MSG: The decision has been recorded as no decision was made regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5610,13 +5610,13 @@
       <c r="C236" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The committee did not reach a decision about the movie to be shown on Friday, so I have recorded a no decision.
 </t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5632,7 +5632,7 @@
       <c r="C237" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for the movie "Barbie."
+MSG: The decision has been recorded, and the movie "Barbie" will be shown on Friday.
 </t>
         </is>
       </c>
@@ -5654,7 +5654,7 @@
       <c r="C238" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown at the event on Friday.
+MSG: The decision to acquire the rights for "Oppenheimer" has been successfully recorded.
 </t>
         </is>
       </c>
@@ -5676,13 +5676,13 @@
       <c r="C239" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been made, and no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5698,7 +5698,7 @@
       <c r="C240" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the screening on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -5720,13 +5720,13 @@
       <c r="C241" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5742,13 +5742,13 @@
       <c r="C242" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer."
+MSG: The decision-making process concluded without a choice for Friday's movie, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5764,13 +5764,13 @@
       <c r="C243" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision process concluded without a definitive choice for Friday's movie, indicating no decision was made.
 </t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5786,13 +5786,13 @@
       <c r="C244" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer," which will be shown on Friday.
+MSG: A decision regarding Friday's movie was not made, so I have recorded a no decision.
 </t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5808,13 +5808,13 @@
       <c r="C245" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded, indicating that no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5830,13 +5830,13 @@
       <c r="C246" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Oppenheimer" on Friday.
+MSG: The decision has been recorded as no decision was reached about which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5852,7 +5852,7 @@
       <c r="C247" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Oppenheimer" for the upcoming event on Friday.
+MSG: The decision to acquire the rights for "Oppenheimer" has been successfully recorded.
 </t>
         </is>
       </c>
@@ -5874,13 +5874,13 @@
       <c r="C248" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5896,13 +5896,13 @@
       <c r="C249" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for the upcoming film showing.
+MSG: The decision about which movie to show on Friday was not reached, leading to the conclusion that no movie will be acquired.
 </t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5918,13 +5918,13 @@
       <c r="C250" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event on Friday.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -5940,13 +5940,13 @@
       <c r="C251" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5962,13 +5962,13 @@
       <c r="C252" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the upcoming event.
+MSG: The decision-making process did not yield a consensus on any specific movie for Friday, leading to the conclusion that no decision can be made at this time.
 </t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -5984,13 +5984,13 @@
       <c r="C253" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about the movie to show on Friday was not made, so no action can be taken.
 </t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6006,13 +6006,13 @@
       <c r="C254" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday could not be made, as there was no agreement reached during the conversation.
 </t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6028,13 +6028,13 @@
       <c r="C255" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision about the movie for Friday has been recorded as "no decision."
 </t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6050,13 +6050,13 @@
       <c r="C256" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to screen "Oppenheimer" for the upcoming event.
+MSG: The decision to select a movie for Friday was not reached, and thus no movie has been acquired.
 </t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6072,13 +6072,13 @@
       <c r="C257" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded with no movie selected.
 </t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6094,13 +6094,13 @@
       <c r="C258" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown at the upcoming event.
+MSG: The decision has been recorded as no movie being chosen for Friday.
 </t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6116,13 +6116,13 @@
       <c r="C259" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no agreement was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6138,13 +6138,13 @@
       <c r="C260" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming screening on Friday.
+MSG: The decision has been recorded as no decision was reached regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6160,7 +6160,7 @@
       <c r="C261" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for the upcoming student assembly.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -6182,13 +6182,13 @@
       <c r="C262" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been recorded as no decision being made regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6204,13 +6204,13 @@
       <c r="C263" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: In this scenario, the conversation ended without a clear decision regarding which movie to show on Friday. Therefore, the appropriate function to call is the no_decision function, indicating that no conclusive choice was made.
 </t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       <c r="C264" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision to acquire the rights for "Barbie" has been confirmed.
 </t>
         </is>
       </c>
@@ -6248,13 +6248,13 @@
       <c r="C265" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights for "Oppenheimer" based on the committee's discussions and the educational value it offers for the students' development.
+MSG: The decision has been recorded as no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6270,13 +6270,13 @@
       <c r="C266" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no agreement was reached regarding the movie selection.
 </t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6292,13 +6292,13 @@
       <c r="C267" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the Friday event.
+MSG: The decision about which movie to acquire for Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6314,7 +6314,7 @@
       <c r="C268" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as "Barbie" being selected for showing on Friday.
 </t>
         </is>
       </c>
@@ -6336,13 +6336,13 @@
       <c r="C269" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for both movies: "Barbie" and "Oppenheimer," as they will be shown in their entirety during the event.
+MSG: The decision process resulted in no agreement on which movie to select for Friday's screening.
 </t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6358,13 +6358,13 @@
       <c r="C270" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Oppenheimer" as the movie to be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6380,13 +6380,13 @@
       <c r="C271" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: No decision was made regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6402,13 +6402,13 @@
       <c r="C272" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the upcoming student event.
+MSG: The decision has been recorded as no decision being made regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6424,13 +6424,13 @@
       <c r="C273" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show *Barbie* on Friday.
+MSG: The decision was made to not select a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6446,7 +6446,7 @@
       <c r="C274" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the rights for "Barbie" will be acquired for the Friday screening.
+MSG: The decision has been made to acquire the rights to show "Barbie" on Friday.
 </t>
         </is>
       </c>
@@ -6468,13 +6468,13 @@
       <c r="C275" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about Friday's movie has not been made.
 </t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6490,7 +6490,7 @@
       <c r="C276" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision has been made to acquire the rights to "Barbie."
 </t>
         </is>
       </c>
@@ -6512,13 +6512,13 @@
       <c r="C277" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no consensus was reached regarding the movie for Friday.
 </t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6534,13 +6534,13 @@
       <c r="C278" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the movie shown on Friday.
+MSG: The committee did not reach a decision about Friday's movie, so the result is that no decision was made.
 </t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6556,7 +6556,7 @@
       <c r="C279" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event on Friday.
+MSG: The decision has been recorded, and the rights for "Barbie" have been acquired.
 </t>
         </is>
       </c>
@@ -6578,13 +6578,13 @@
       <c r="C280" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision regarding which movie to show on Friday has not been made.
 </t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6600,13 +6600,13 @@
       <c r="C281" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded as no decision about Friday’s movie can be made at this time.
 </t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6622,13 +6622,13 @@
       <c r="C282" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The decision about which movie to show on Friday could not be reached.
 </t>
         </is>
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6644,13 +6644,13 @@
       <c r="C283" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision-making process ended without a definitive choice for Friday's movie, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6666,7 +6666,7 @@
       <c r="C284" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and the rights to "Barbie" will be acquired for the screening.
 </t>
         </is>
       </c>
@@ -6688,13 +6688,13 @@
       <c r="C285" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday could not be made.
 </t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6710,13 +6710,13 @@
       <c r="C286" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have decided to acquire the rights to "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded that no movie will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6732,13 +6732,13 @@
       <c r="C287" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the assembly on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6754,7 +6754,7 @@
       <c r="C288" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for both movies, "Barbie" and "Oppenheimer," as the committee agreed to showcase both films at the event.
+MSG: I have successfully acquired the rights to both movies for Friday's showing.
 </t>
         </is>
       </c>
@@ -6776,13 +6776,13 @@
       <c r="C289" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for Friday's screening.
+MSG: The decision about which movie to show on Friday has not been reached.
 </t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6798,13 +6798,13 @@
       <c r="C290" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no movie was selected for Friday.
 </t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6820,13 +6820,13 @@
       <c r="C291" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as no decision.
 </t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6842,7 +6842,7 @@
       <c r="C292" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision to show "Oppenheimer" has been successfully recorded.
 </t>
         </is>
       </c>
@@ -6864,13 +6864,13 @@
       <c r="C293" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision regarding the movie selection for Friday has not been made, resulting in no acquisition of movie rights at this time.
 </t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6886,7 +6886,7 @@
       <c r="C294" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" as the film to be shown at the school event.
+MSG: The decision to acquire the rights for "Oppenheimer" has been made.
 </t>
         </is>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="C295" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has decided to acquire the rights to show "Barbie" for the event on Friday.
+MSG: The decision to show "Barbie" on Friday has been recorded successfully.
 </t>
         </is>
       </c>
@@ -6930,13 +6930,13 @@
       <c r="C296" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision about which movie to show on Friday has concluded without a selection being made.
 </t>
         </is>
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6952,13 +6952,13 @@
       <c r="C297" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -6974,13 +6974,13 @@
       <c r="C298" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for the movie "Barbie."
+MSG: The decision has been recorded, and the rights for both movies will be acquired.
 </t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -6996,13 +6996,13 @@
       <c r="C299" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the upcoming event.
+MSG: No decision was reached in this meeting regarding the selection of "Oppenheimer" or "Barbie."
 </t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7018,7 +7018,7 @@
       <c r="C300" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Oppenheimer."
+MSG: The decision to acquire the rights for "Oppenheimer" has been successfully made.
 </t>
         </is>
       </c>
@@ -7040,13 +7040,13 @@
       <c r="C301" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision was made not to select a movie for Friday.
 </t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7062,13 +7062,13 @@
       <c r="C302" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been recorded, and no movie will be acquired for screening on Friday.
 </t>
         </is>
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7084,13 +7084,13 @@
       <c r="C303" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for “Oppenheimer” for the Friday movie showing.
+MSG: The decision-making process concluded without a clear agreement on the movie selection, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7106,13 +7106,13 @@
       <c r="C304" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the screening on Friday.
+MSG: The decision about which movie to play on Friday remains unresolved, so no action has been taken.
 </t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7128,7 +7128,7 @@
       <c r="C305" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision to acquire the rights for "Barbie" has been made.
 </t>
         </is>
       </c>
@@ -7150,7 +7150,7 @@
       <c r="C306" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -7172,13 +7172,13 @@
       <c r="C307" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" based on the committee's discussions and agreements.
+MSG: The rights for both movies have been acquired successfully.
 </t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -7194,13 +7194,13 @@
       <c r="C308" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" for the scheduled viewing.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -7216,13 +7216,13 @@
       <c r="C309" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming event.
+MSG: The conversation ended without a mutual decision about which movie to show on Friday, so no action has been taken regarding the acquisition of movie rights.
 </t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7238,13 +7238,13 @@
       <c r="C310" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie" for the movie shown on Friday.
+MSG: The decision about which movie to show on Friday was not made.
 </t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -7260,13 +7260,13 @@
       <c r="C311" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Oppenheimer" for Friday's movie event.
+MSG: The decision has been recorded, and no specific movie will be acquired at this time.
 </t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>

</xml_diff>